<commit_message>
More tests and coverage
</commit_message>
<xml_diff>
--- a/media/test_imports/with_extra_fields_and_group.xlsx
+++ b/media/test_imports/with_extra_fields_and_group.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>URN:Tel</t>
   </si>
@@ -19,6 +19,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>language</t>
+  </si>
+  <si>
     <t>Created On</t>
   </si>
   <si>
@@ -37,6 +40,9 @@
     <t>John Doe</t>
   </si>
   <si>
+    <t>eng</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
@@ -44,6 +50,9 @@
   </si>
   <si>
     <t>Mary Smith</t>
+  </si>
+  <si>
+    <t>spa</t>
   </si>
   <si>
     <t>+250788456678</t>
@@ -1253,7 +1262,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1261,11 +1270,11 @@
   <cols>
     <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.3516" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1287,57 +1296,67 @@
       <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
         <v>44091</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" t="s" s="2">
-        <v>8</v>
+      <c r="G2" t="s" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5">
         <v>43961</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="5">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
         <v>43993</v>
       </c>
-      <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" t="s" s="2">
-        <v>12</v>
+      <c r="F4" s="6"/>
+      <c r="G4" t="s" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="5" ht="15.35" customHeight="1">
@@ -1347,6 +1366,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" s="6"/>
@@ -1355,6 +1375,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" s="6"/>
@@ -1363,6 +1384,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="6"/>
@@ -1371,6 +1393,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="6"/>
@@ -1379,6 +1402,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="6"/>
@@ -1387,6 +1411,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>